<commit_message>
updated unit test protocol
</commit_message>
<xml_diff>
--- a/Unit Test Protocol (Moving Car).xlsx
+++ b/Unit Test Protocol (Moving Car).xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>Task Status</t>
   </si>
@@ -121,6 +121,51 @@
   </si>
   <si>
     <t>Application (car_cycle() function)</t>
+  </si>
+  <si>
+    <t>Call TIMER0_delay(3000) to delay the code for 3 seconds</t>
+  </si>
+  <si>
+    <t>delay 3 seconds</t>
+  </si>
+  <si>
+    <t>code is delayed for 3 seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call MOTOR_control(enable pin,port number,duty cycle) </t>
+  </si>
+  <si>
+    <t>car should move at 50% speed</t>
+  </si>
+  <si>
+    <t>car moves at 50% speed</t>
+  </si>
+  <si>
+    <t>call car_cycle() the main application</t>
+  </si>
+  <si>
+    <t>car keeps looping over the states</t>
+  </si>
+  <si>
+    <t>car kept looping over the states</t>
+  </si>
+  <si>
+    <t>call BUTTON_read(pin number, port number) to turn on led</t>
+  </si>
+  <si>
+    <t>led should turn on</t>
+  </si>
+  <si>
+    <t>led turned on</t>
+  </si>
+  <si>
+    <t>call LED_toggle(pin number, port number)</t>
+  </si>
+  <si>
+    <t>led should toggle</t>
+  </si>
+  <si>
+    <t>led keep toggling</t>
   </si>
 </sst>
 </file>
@@ -472,7 +517,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +612,15 @@
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="G4" s="6" t="s">
         <v>20</v>
       </c>
@@ -582,7 +635,15 @@
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="G5" s="6" t="s">
         <v>20</v>
       </c>
@@ -597,7 +658,15 @@
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="D6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="G6" s="6" t="s">
         <v>20</v>
       </c>
@@ -612,7 +681,15 @@
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="D7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="G7" s="6" t="s">
         <v>20</v>
       </c>
@@ -627,7 +704,15 @@
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="D8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="G8" s="6" t="s">
         <v>20</v>
       </c>
@@ -642,7 +727,15 @@
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="G9" s="6" t="s">
         <v>20</v>
       </c>

</xml_diff>